<commit_message>
added i2c to ext connector
</commit_message>
<xml_diff>
--- a/PCB/BOM/AssemblyTOP_BOT.xlsx
+++ b/PCB/BOM/AssemblyTOP_BOT.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C34C4B3B-6CD6-4840-9005-3593ACBB01DA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{CD044FB2-0955-4B30-A464-13B7B507D34E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3630" yWindow="1410" windowWidth="28485" windowHeight="12840" xr2:uid="{364517D3-982F-4BC2-8D6A-0BB8872C8EF2}"/>
+    <workbookView xWindow="3630" yWindow="1410" windowWidth="28485" windowHeight="12840" xr2:uid="{F9BE8ECC-2852-4772-93D5-63BAC6B01681}"/>
   </bookViews>
   <sheets>
     <sheet name="AssemblyTOP_BOT" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="541" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="241">
   <si>
     <t>Layer</t>
   </si>
@@ -379,7 +379,7 @@
     <t>1469743</t>
   </si>
   <si>
-    <t>R29, R43</t>
+    <t>R29, R43, R56</t>
   </si>
   <si>
     <t>0</t>
@@ -511,6 +511,21 @@
     <t>2356131</t>
   </si>
   <si>
+    <t>Not Fitted</t>
+  </si>
+  <si>
+    <t>R57</t>
+  </si>
+  <si>
+    <t>1k</t>
+  </si>
+  <si>
+    <t>CRCW06031K00FKEA</t>
+  </si>
+  <si>
+    <t>1469740</t>
+  </si>
+  <si>
     <t>Bottom</t>
   </si>
   <si>
@@ -643,103 +658,97 @@
     <t>1652885</t>
   </si>
   <si>
-    <t>R34, R35, R40, R41, R44, R45, R52</t>
-  </si>
-  <si>
-    <t>1k</t>
-  </si>
-  <si>
-    <t>CRCW06031K00FKEA</t>
-  </si>
-  <si>
-    <t>1469740</t>
+    <t>R34, R35, R41, R44, R45, R52</t>
+  </si>
+  <si>
+    <t>R4, R40, R58</t>
+  </si>
+  <si>
+    <t>115k</t>
+  </si>
+  <si>
+    <t>CRCW0603115KFKEA</t>
+  </si>
+  <si>
+    <t>2138503</t>
+  </si>
+  <si>
+    <t>R5, R6</t>
+  </si>
+  <si>
+    <t>25k5</t>
+  </si>
+  <si>
+    <t>CRCW060325K5FKEA</t>
+  </si>
+  <si>
+    <t>2138447</t>
+  </si>
+  <si>
+    <t>R7, R54, R55</t>
+  </si>
+  <si>
+    <t>R8</t>
+  </si>
+  <si>
+    <t>U1</t>
+  </si>
+  <si>
+    <t>LTC3622HDE-2#PBF</t>
+  </si>
+  <si>
+    <t>DFN-14</t>
+  </si>
+  <si>
+    <t>Buck, 2 Channel, 2.25MHz</t>
+  </si>
+  <si>
+    <t>2483300</t>
+  </si>
+  <si>
+    <t>U4, U5</t>
+  </si>
+  <si>
+    <t>SN74LVC2T45DCTR</t>
+  </si>
+  <si>
+    <t>SSOP-8_DCT</t>
+  </si>
+  <si>
+    <t>2854638</t>
+  </si>
+  <si>
+    <t>Y1</t>
+  </si>
+  <si>
+    <t>ABM3B-8.000MHZ-10-1-U-T</t>
+  </si>
+  <si>
+    <t>XTAL_5X3.2MM</t>
+  </si>
+  <si>
+    <t>8MHz, 10ppm, 10pF</t>
+  </si>
+  <si>
+    <t>2467817</t>
+  </si>
+  <si>
+    <t>Fitted, Not Fitted, Fitted, Fitted, Not Fitted, Fitted, Fitted, Not Fitted, Fitted, Not Fitted, Fitted, Fitted, Fitted</t>
+  </si>
+  <si>
+    <t>R1, R2, R17, R18, R19, R20, R21, R22, R23, R24, R32, R33, R50</t>
+  </si>
+  <si>
+    <t>Fitted, Not Fitted, Not Fitted</t>
+  </si>
+  <si>
+    <t>FB1, FB5, FB6</t>
+  </si>
+  <si>
+    <t>Not Fitted, Fitted, Fitted, Fitted, Fitted, Fitted</t>
   </si>
   <si>
     <t>R36, R38, R46, R47, R51, R53</t>
-  </si>
-  <si>
-    <t>R4</t>
-  </si>
-  <si>
-    <t>115k</t>
-  </si>
-  <si>
-    <t>CRCW0603115KFKEA</t>
-  </si>
-  <si>
-    <t>2138503</t>
-  </si>
-  <si>
-    <t>R5, R6</t>
-  </si>
-  <si>
-    <t>25k5</t>
-  </si>
-  <si>
-    <t>CRCW060325K5FKEA</t>
-  </si>
-  <si>
-    <t>2138447</t>
-  </si>
-  <si>
-    <t>R7</t>
-  </si>
-  <si>
-    <t>R8</t>
-  </si>
-  <si>
-    <t>U1</t>
-  </si>
-  <si>
-    <t>LTC3622HDE-2#PBF</t>
-  </si>
-  <si>
-    <t>DFN-14</t>
-  </si>
-  <si>
-    <t>Buck, 2 Channel, 2.25MHz</t>
-  </si>
-  <si>
-    <t>2483300</t>
-  </si>
-  <si>
-    <t>U4, U5</t>
-  </si>
-  <si>
-    <t>SN74LVC2T45DCTR</t>
-  </si>
-  <si>
-    <t>SSOP-8_DCT</t>
-  </si>
-  <si>
-    <t>2854638</t>
-  </si>
-  <si>
-    <t>Y1</t>
-  </si>
-  <si>
-    <t>ABM3B-8.000MHZ-10-1-U-T</t>
-  </si>
-  <si>
-    <t>XTAL_5X3.2MM</t>
-  </si>
-  <si>
-    <t>8MHz, 10ppm, 10pF</t>
-  </si>
-  <si>
-    <t>2467817</t>
-  </si>
-  <si>
-    <t>Fitted, Not Fitted, Fitted, Fitted, Not Fitted, Fitted, Fitted, Not Fitted, Fitted, Not Fitted, Fitted, Fitted, Fitted</t>
-  </si>
-  <si>
-    <t>R1, R2, R17, R18, R19, R20, R21, R22, R23, R24, R32, R33, R50</t>
-  </si>
-  <si>
-    <t>Fitted, Not Fitted, Not Fitted</t>
-  </si>
-  <si>
-    <t>FB1, FB5, FB6</t>
   </si>
 </sst>
 </file>
@@ -1122,8 +1131,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AEF0048C-692D-462F-A803-2775CAA93633}">
-  <dimension ref="A1:J60"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE5A521B-5131-4E59-AAD7-37CA86A16C92}">
+  <dimension ref="A1:J61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1891,7 +1900,7 @@
         <v>118</v>
       </c>
       <c r="E24" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F24" s="2" t="s">
         <v>119</v>
@@ -2199,31 +2208,31 @@
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B34" s="2" t="s">
         <v>161</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>1</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>162</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>12</v>
+        <v>163</v>
       </c>
       <c r="E34" s="3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>13</v>
+        <v>164</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>14</v>
+        <v>63</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>15</v>
+        <v>115</v>
       </c>
       <c r="I34" s="2" t="s">
-        <v>16</v>
+        <v>165</v>
       </c>
       <c r="J34" s="2" t="s">
         <v>17</v>
@@ -2231,31 +2240,31 @@
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="E35" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="G35" s="2" t="s">
         <v>14</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="I35" s="2" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
       <c r="J35" s="2" t="s">
         <v>17</v>
@@ -2263,31 +2272,31 @@
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>165</v>
+        <v>30</v>
       </c>
       <c r="E36" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>166</v>
+        <v>31</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>167</v>
+        <v>14</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>168</v>
+        <v>32</v>
       </c>
       <c r="I36" s="2" t="s">
-        <v>169</v>
+        <v>33</v>
       </c>
       <c r="J36" s="2" t="s">
         <v>17</v>
@@ -2295,31 +2304,31 @@
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C37" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="D37" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="D37" s="2" t="s">
+      <c r="E37" s="3">
+        <v>3</v>
+      </c>
+      <c r="F37" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="E37" s="3">
-        <v>2</v>
-      </c>
-      <c r="F37" s="2" t="s">
+      <c r="G37" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="G37" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="H37" s="2" t="s">
-        <v>21</v>
+        <v>173</v>
       </c>
       <c r="I37" s="2" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="J37" s="2" t="s">
         <v>17</v>
@@ -2327,31 +2336,31 @@
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="E38" s="3">
         <v>2</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>177</v>
+        <v>14</v>
       </c>
       <c r="H38" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I38" s="2" t="s">
         <v>178</v>
-      </c>
-      <c r="I38" s="2" t="s">
-        <v>179</v>
       </c>
       <c r="J38" s="2" t="s">
         <v>17</v>
@@ -2359,31 +2368,31 @@
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C39" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="D39" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="D39" s="2" t="s">
-        <v>19</v>
-      </c>
       <c r="E39" s="3">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>20</v>
+        <v>181</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>14</v>
+        <v>182</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>21</v>
+        <v>183</v>
       </c>
       <c r="I39" s="2" t="s">
-        <v>22</v>
+        <v>184</v>
       </c>
       <c r="J39" s="2" t="s">
         <v>17</v>
@@ -2391,31 +2400,31 @@
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="E40" s="3">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="G40" s="2" t="s">
         <v>14</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="I40" s="2" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="J40" s="2" t="s">
         <v>17</v>
@@ -2423,31 +2432,31 @@
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="B41" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="E41" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>57</v>
+        <v>36</v>
       </c>
       <c r="G41" s="2" t="s">
-        <v>58</v>
+        <v>14</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>59</v>
+        <v>37</v>
       </c>
       <c r="I41" s="2" t="s">
-        <v>60</v>
+        <v>38</v>
       </c>
       <c r="J41" s="2" t="s">
         <v>17</v>
@@ -2455,31 +2464,31 @@
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="B42" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>184</v>
+        <v>28</v>
       </c>
       <c r="E42" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>185</v>
+        <v>57</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>186</v>
+        <v>58</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>187</v>
+        <v>59</v>
       </c>
       <c r="I42" s="2" t="s">
-        <v>188</v>
+        <v>60</v>
       </c>
       <c r="J42" s="2" t="s">
         <v>17</v>
@@ -2487,31 +2496,31 @@
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="B43" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C43" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="D43" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="D43" s="2" t="s">
+      <c r="E43" s="3">
+        <v>1</v>
+      </c>
+      <c r="F43" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="E43" s="3">
-        <v>1</v>
-      </c>
-      <c r="F43" s="2" t="s">
+      <c r="G43" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="G43" s="2" t="s">
-        <v>186</v>
-      </c>
       <c r="H43" s="2" t="s">
-        <v>187</v>
+        <v>192</v>
       </c>
       <c r="I43" s="2" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="J43" s="2" t="s">
         <v>17</v>
@@ -2519,31 +2528,31 @@
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="B44" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>28</v>
+        <v>195</v>
       </c>
       <c r="E44" s="3">
         <v>1</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>85</v>
+        <v>196</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>86</v>
+        <v>191</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>28</v>
+        <v>192</v>
       </c>
       <c r="I44" s="2" t="s">
-        <v>87</v>
+        <v>197</v>
       </c>
       <c r="J44" s="2" t="s">
         <v>17</v>
@@ -2551,13 +2560,13 @@
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="D45" s="2" t="s">
         <v>28</v>
@@ -2566,16 +2575,16 @@
         <v>1</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="G45" s="2" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="H45" s="2" t="s">
         <v>28</v>
       </c>
       <c r="I45" s="2" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="J45" s="2" t="s">
         <v>17</v>
@@ -2583,31 +2592,31 @@
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="B46" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>98</v>
+        <v>28</v>
       </c>
       <c r="E46" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="G46" s="2" t="s">
-        <v>63</v>
+        <v>90</v>
       </c>
       <c r="H46" s="2" t="s">
-        <v>95</v>
+        <v>28</v>
       </c>
       <c r="I46" s="2" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="J46" s="2" t="s">
         <v>17</v>
@@ -2615,22 +2624,22 @@
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="B47" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="E47" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="G47" s="2" t="s">
         <v>63</v>
@@ -2639,7 +2648,7 @@
         <v>95</v>
       </c>
       <c r="I47" s="2" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="J47" s="2" t="s">
         <v>17</v>
@@ -2647,31 +2656,31 @@
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="B48" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>198</v>
+        <v>102</v>
       </c>
       <c r="E48" s="3">
         <v>1</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>199</v>
+        <v>103</v>
       </c>
       <c r="G48" s="2" t="s">
         <v>63</v>
       </c>
       <c r="H48" s="2" t="s">
-        <v>115</v>
+        <v>95</v>
       </c>
       <c r="I48" s="2" t="s">
-        <v>200</v>
+        <v>104</v>
       </c>
       <c r="J48" s="2" t="s">
         <v>17</v>
@@ -2679,22 +2688,22 @@
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="B49" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="E49" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="G49" s="2" t="s">
         <v>63</v>
@@ -2703,7 +2712,7 @@
         <v>115</v>
       </c>
       <c r="I49" s="2" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="J49" s="2" t="s">
         <v>17</v>
@@ -2711,22 +2720,22 @@
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="B50" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="E50" s="3">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="G50" s="2" t="s">
         <v>63</v>
@@ -2735,7 +2744,7 @@
         <v>115</v>
       </c>
       <c r="I50" s="2" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="J50" s="2" t="s">
         <v>17</v>
@@ -2743,22 +2752,22 @@
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="B51" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>118</v>
+        <v>163</v>
       </c>
       <c r="E51" s="3">
         <v>6</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>119</v>
+        <v>164</v>
       </c>
       <c r="G51" s="2" t="s">
         <v>63</v>
@@ -2767,7 +2776,7 @@
         <v>115</v>
       </c>
       <c r="I51" s="2" t="s">
-        <v>120</v>
+        <v>165</v>
       </c>
       <c r="J51" s="2" t="s">
         <v>17</v>
@@ -2775,22 +2784,22 @@
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="B52" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="E52" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="G52" s="2" t="s">
         <v>63</v>
@@ -2799,7 +2808,7 @@
         <v>115</v>
       </c>
       <c r="I52" s="2" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="J52" s="2" t="s">
         <v>17</v>
@@ -2807,22 +2816,22 @@
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="B53" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="E53" s="3">
         <v>2</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="G53" s="2" t="s">
         <v>63</v>
@@ -2831,7 +2840,7 @@
         <v>115</v>
       </c>
       <c r="I53" s="2" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="J53" s="2" t="s">
         <v>17</v>
@@ -2839,19 +2848,19 @@
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="B54" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="D54" s="2" t="s">
         <v>93</v>
       </c>
       <c r="E54" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F54" s="2" t="s">
         <v>94</v>
@@ -2871,13 +2880,13 @@
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="B55" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="D55" s="2" t="s">
         <v>126</v>
@@ -2903,13 +2912,13 @@
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="B56" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="D56" s="2" t="s">
         <v>28</v>
@@ -2918,16 +2927,16 @@
         <v>1</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="G56" s="2" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="H56" s="2" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="I56" s="2" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="J56" s="2" t="s">
         <v>17</v>
@@ -2935,13 +2944,13 @@
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="B57" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="D57" s="2" t="s">
         <v>28</v>
@@ -2950,16 +2959,16 @@
         <v>2</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="G57" s="2" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="H57" s="2" t="s">
         <v>28</v>
       </c>
       <c r="I57" s="2" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="J57" s="2" t="s">
         <v>17</v>
@@ -2967,13 +2976,13 @@
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="B58" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D58" s="2" t="s">
         <v>28</v>
@@ -2982,16 +2991,16 @@
         <v>1</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="G58" s="2" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="H58" s="2" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="I58" s="2" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="J58" s="2" t="s">
         <v>17</v>
@@ -2999,13 +3008,13 @@
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="D59" s="2" t="s">
         <v>72</v>
@@ -3031,13 +3040,13 @@
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="D60" s="2" t="s">
         <v>28</v>
@@ -3058,6 +3067,38 @@
         <v>70</v>
       </c>
       <c r="J60" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A61" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="E61" s="3">
+        <v>5</v>
+      </c>
+      <c r="F61" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="G61" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="H61" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="I61" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="J61" s="2" t="s">
         <v>17</v>
       </c>
     </row>

</xml_diff>